<commit_message>
Unnötige Excel Date gelöscht.
</commit_message>
<xml_diff>
--- a/0-Datengrundlage/1-Sponsoren/Sponsoren - Bezeichnung.xlsx
+++ b/0-Datengrundlage/1-Sponsoren/Sponsoren - Bezeichnung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tricuper\Documents\GitHub\Sponsorendatenbank\0-Datengrundlage\1-Sponsoren\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9226A7FA-ECF6-4755-A705-9F9952C472D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38809570-1581-4770-9D6B-3BD37F54262B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -552,7 +552,7 @@
   <dimension ref="A1:B68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C69"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>